<commit_message>
Cleaned up naming throughout, refactored common controller code
</commit_message>
<xml_diff>
--- a/apodeixi/controllers/kernel/bdd/test_unit/input_data/feature_injection_INPUT.xlsx
+++ b/apodeixi/controllers/kernel/bdd/test_unit/input_data/feature_injection_INPUT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\documentation\kernel-knowledge-base\excel-postings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\apodeixi\controllers\kernel\bdd\test_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671B9798-9478-4936-8F2B-C3D2042AA489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA707438-0F3D-4A49-9D1A-AE72899831ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{4B727691-5255-46C4-A89F-234F9FDCAFEC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="118">
   <si>
     <t>Journeys</t>
   </si>
@@ -304,85 +304,91 @@
     <t>BDD</t>
   </si>
   <si>
-    <t>Context</t>
-  </si>
-  <si>
     <t>environment</t>
   </si>
   <si>
     <t>Production</t>
   </si>
   <si>
+    <t>Apodeixi BDD tests</t>
+  </si>
+  <si>
+    <t>BDD Scaffolding</t>
+  </si>
+  <si>
+    <t>alejandro@chateauclaudia-labs.com</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>projectType</t>
+  </si>
+  <si>
+    <t>dataRange</t>
+  </si>
+  <si>
+    <t>"what'</t>
+  </si>
+  <si>
+    <t>"why"</t>
+  </si>
+  <si>
+    <t>"who"</t>
+  </si>
+  <si>
+    <t>"how"</t>
+  </si>
+  <si>
+    <t>"scenarios"</t>
+  </si>
+  <si>
+    <t>Jobs to be done</t>
+  </si>
+  <si>
+    <t>Stakeholders</t>
+  </si>
+  <si>
+    <t>Capabilities</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>DDD Aggregate</t>
+  </si>
+  <si>
+    <t>DDD sub domain</t>
+  </si>
+  <si>
+    <t>DDD Bounded Context</t>
+  </si>
+  <si>
+    <t>Manifest</t>
+  </si>
+  <si>
+    <t>Function(s)</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>E5:I100</t>
+  </si>
+  <si>
+    <t>excelAPI</t>
+  </si>
+  <si>
+    <t>capability-hierarchy.kernel.a6i.xlsx/v1a</t>
+  </si>
+  <si>
+    <t>Posting Label</t>
+  </si>
+  <si>
     <t>recordedBy</t>
-  </si>
-  <si>
-    <t>Apodeixi BDD tests</t>
-  </si>
-  <si>
-    <t>BDD Scaffolding</t>
-  </si>
-  <si>
-    <t>alejandro@chateauclaudia-labs.com</t>
-  </si>
-  <si>
-    <t>projectName</t>
-  </si>
-  <si>
-    <t>projectType</t>
-  </si>
-  <si>
-    <t>dataRange</t>
-  </si>
-  <si>
-    <t>"what'</t>
-  </si>
-  <si>
-    <t>"why"</t>
-  </si>
-  <si>
-    <t>"who"</t>
-  </si>
-  <si>
-    <t>"how"</t>
-  </si>
-  <si>
-    <t>"scenarios"</t>
-  </si>
-  <si>
-    <t>Jobs to be done</t>
-  </si>
-  <si>
-    <t>Stakeholders</t>
-  </si>
-  <si>
-    <t>Capabilities</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>DDD Aggregate</t>
-  </si>
-  <si>
-    <t>DDD sub domain</t>
-  </si>
-  <si>
-    <t>DDD Bounded Context</t>
-  </si>
-  <si>
-    <t>Manifest</t>
-  </si>
-  <si>
-    <t>Function(s)</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>E5:I100</t>
   </si>
 </sst>
 </file>
@@ -518,6 +524,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -526,33 +559,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,12 +890,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -1103,7 +1109,7 @@
   <dimension ref="B1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1122,113 +1128,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="B1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B2" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="K3" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="B4" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="E4" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="E5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>74</v>
@@ -1237,7 +1247,7 @@
         <v>76</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>67</v>
@@ -1246,18 +1256,18 @@
         <v>79</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:17" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B6" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>95</v>
+      <c r="B6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>81</v>
@@ -1298,11 +1308,11 @@
       </c>
     </row>
     <row r="7" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>115</v>
+      <c r="B7" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1321,8 +1331,8 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="2:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
       <c r="E8" s="2" t="s">
         <v>62</v>
       </c>
@@ -1361,8 +1371,8 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="M9" s="2" t="s">
         <v>68</v>
       </c>
@@ -1377,22 +1387,22 @@
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="I10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B11" s="15"/>
-      <c r="C11" s="17"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="14"/>
       <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B12" s="15"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="15"/>
       <c r="H12" s="2" t="s">
         <v>72</v>
       </c>
@@ -1404,8 +1414,8 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B13" s="15"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="14"/>
       <c r="I13" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>